<commit_message>
Add NewRelic, modify data type of stars and bookeddates data sent to React app
</commit_message>
<xml_diff>
--- a/Speed Tracking.xlsx
+++ b/Speed Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showObjects="placeholders" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25540" windowHeight="12280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25540" windowHeight="11440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Mongo</t>
   </si>
@@ -57,7 +57,16 @@
     <t>Write (ms, avg of 1000)</t>
   </si>
   <si>
-    <t>Fetch (ms, avg of 1000)</t>
+    <t>Fetch sequential ORM (ms, avg of 1000)</t>
+  </si>
+  <si>
+    <t>Fetch sequential raw/native</t>
+  </si>
+  <si>
+    <t>Fetch simultaneous ORM</t>
+  </si>
+  <si>
+    <t>Fetch simultaneous raw</t>
   </si>
 </sst>
 </file>
@@ -124,7 +133,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -140,6 +149,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -147,7 +158,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -155,12 +166,14 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
   </cellStyles>
@@ -491,10 +504,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -504,10 +518,13 @@
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="24" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -527,10 +544,19 @@
         <v>12</v>
       </c>
       <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -549,13 +575,18 @@
         <v>-0.30706346153846159</v>
       </c>
       <c r="G2" s="3">
-        <v>3.7080000000000002</v>
+        <v>4.3040000000000003</v>
       </c>
       <c r="H2" s="3">
-        <v>8.4510000000000005</v>
+        <v>3.1680000000000001</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3">
+        <v>9.9890000000000008</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -565,13 +596,18 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3">
-        <v>2.5950000000000002</v>
+        <v>5.0430000000000001</v>
       </c>
       <c r="H3" s="3">
-        <v>1.587</v>
+        <v>5.306</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3">
+        <v>1.736</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -581,13 +617,18 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="3">
-        <v>3.2519999999999998</v>
+        <v>4.109</v>
       </c>
       <c r="H4" s="3">
-        <v>5.66</v>
+        <v>4.2350000000000003</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3">
+        <v>6.3150000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -607,22 +648,24 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="3">
-        <f>SUM(G3:G4)</f>
-        <v>5.8469999999999995</v>
+        <v>9.1519999999999992</v>
       </c>
       <c r="H5" s="3">
-        <f>SUM(H3:H4)</f>
-        <v>7.2469999999999999</v>
+        <v>9.5410000000000004</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3.242</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3.1520000000000001</v>
+      </c>
+      <c r="K5" s="3">
+        <v>8.0510000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="D6" s="1">
-        <v>8253882</v>
-      </c>
-      <c r="E6" s="1">
-        <f>D6/1000/60</f>
-        <v>137.56469999999999</v>
-      </c>
+    <row r="6" spans="1:11">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add stress testing and psql autoincrement reset due to batch insert glitch
</commit_message>
<xml_diff>
--- a/Speed Tracking.xlsx
+++ b/Speed Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showObjects="placeholders" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25540" windowHeight="11440" tabRatio="500"/>
+    <workbookView xWindow="1540" yWindow="4660" windowWidth="25540" windowHeight="11440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -575,15 +575,15 @@
         <v>-0.30706346153846159</v>
       </c>
       <c r="G2" s="3">
-        <v>4.3040000000000003</v>
+        <v>3.3071999999999999</v>
       </c>
       <c r="H2" s="3">
-        <v>3.1680000000000001</v>
+        <v>2.3847999999999998</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3">
-        <v>9.9890000000000008</v>
+        <v>10.4026</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -596,15 +596,15 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3">
-        <v>5.0430000000000001</v>
+        <v>3.649</v>
       </c>
       <c r="H3" s="3">
-        <v>5.306</v>
+        <v>3.9079999999999999</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3">
-        <v>1.736</v>
+        <v>2.2360000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -617,15 +617,15 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="3">
-        <v>4.109</v>
+        <v>3.9660000000000002</v>
       </c>
       <c r="H4" s="3">
-        <v>4.2350000000000003</v>
+        <v>4.3912000000000004</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3">
-        <v>6.3150000000000004</v>
+        <v>7.0288000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -648,19 +648,19 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="3">
-        <v>9.1519999999999992</v>
+        <v>7.6158000000000001</v>
       </c>
       <c r="H5" s="3">
-        <v>9.5410000000000004</v>
+        <v>8.2992000000000008</v>
       </c>
       <c r="I5" s="3">
-        <v>3.242</v>
+        <v>4.3920000000000003</v>
       </c>
       <c r="J5" s="3">
-        <v>3.1520000000000001</v>
+        <v>3.6814</v>
       </c>
       <c r="K5" s="3">
-        <v>8.0510000000000002</v>
+        <v>9.2639999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:11">

</xml_diff>